<commit_message>
LogBook, BackLog & BurndownChart
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="1" r:id="rId1"/>
     <sheet name="Initial" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
   <si>
     <t>Sprint</t>
   </si>
@@ -113,6 +114,9 @@
   </si>
   <si>
     <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
   </si>
 </sst>
 </file>
@@ -190,10 +194,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,6 +343,97 @@
         <a:xfrm>
           <a:off x="6696074" y="666749"/>
           <a:ext cx="5534025" cy="4432665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>11142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="6998"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="704850"/>
+          <a:ext cx="5505450" cy="4430742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>153779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="6859"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6712725" y="657225"/>
+          <a:ext cx="5488800" cy="4430504"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -628,19 +723,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -770,28 +865,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
     </row>
     <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -953,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,28 +1058,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
     </row>
     <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1117,6 +1212,186 @@
       </c>
       <c r="C40" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="O47" s="3"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="O78" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:R2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="2">
+        <v>2</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="2">
+        <v>3</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32" s="2">
+        <v>4</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="2">
+        <v>5</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="2">
+        <v>6</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>7</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="2">
+        <v>7</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" s="2">
+        <v>8</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Log Book D - 9
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="1" r:id="rId1"/>
     <sheet name="Initial" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 1" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 2" sheetId="5" r:id="rId4"/>
+    <sheet name="Sprint 3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="31">
   <si>
     <t>Sprint</t>
   </si>
@@ -117,6 +118,9 @@
   </si>
   <si>
     <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
   </si>
 </sst>
 </file>
@@ -194,10 +198,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,6 +438,97 @@
         <a:xfrm>
           <a:off x="6712725" y="657225"/>
           <a:ext cx="5488800" cy="4430504"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167865</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="6418"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="657225"/>
+          <a:ext cx="5476875" cy="4444590"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>447675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>16649</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>103992</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="7648"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6734174" y="638175"/>
+          <a:ext cx="5474475" cy="4399767"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -723,19 +818,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -865,28 +960,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1058,28 +1153,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1236,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
@@ -1246,28 +1341,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1392,6 +1487,194 @@
       </c>
       <c r="M36" s="2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="O47" s="3"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="O78" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:R2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30" s="2">
+        <v>2</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="2">
+        <v>3</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" s="2">
+        <v>4</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L33" s="2">
+        <v>5</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L34" s="2">
+        <v>6</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L35" s="2">
+        <v>7</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L36" s="2">
+        <v>8</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L37" s="2">
+        <v>9</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L38" s="2">
+        <v>10</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L39" s="2">
+        <v>11</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L40" s="2">
+        <v>12</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Log Book D -12
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\Semester 4\Teknik Kolaborasi PL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\C\MoonLightTrinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sprint 1" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 2" sheetId="5" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="6" r:id="rId5"/>
+    <sheet name="Sprint 4" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
   <si>
     <t>Sprint</t>
   </si>
@@ -540,6 +541,97 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167865</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="7220"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="695325"/>
+          <a:ext cx="5514975" cy="4406490"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>7124</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1378</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="6659"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705599" y="685799"/>
+          <a:ext cx="5493525" cy="4440029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1511,7 +1603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
@@ -1693,4 +1785,200 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="5" spans="2:18" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="2">
+        <v>2</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="2">
+        <v>3</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="2">
+        <v>4</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L33" s="2">
+        <v>5</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L34" s="2">
+        <v>6</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L35" s="2">
+        <v>7</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L36" s="2">
+        <v>8</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L37" s="2">
+        <v>9</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L38" s="2">
+        <v>10</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L39" s="2">
+        <v>11</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L40" s="2">
+        <v>12</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L41" s="2">
+        <v>13</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L42" s="2">
+        <v>14</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L43" s="2">
+        <v>15</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L44" s="2">
+        <v>16</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="O47" s="3"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="O78" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:R2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>